<commit_message>
New Keys for answers S, L and Space S: no detection L: detection Space: replay
</commit_message>
<xml_diff>
--- a/stories/Bunny/story.xlsx
+++ b/stories/Bunny/story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheylus/Documents/Rita/MLPstory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheylus/Documents/Rita/PythonMLP_2024_PAMCAP_EPCT_Rita/stories/Bunny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684AC177-8F3B-AF45-9B26-2678919CFEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F63282-B743-304B-9586-463C33DF2508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="4760" windowWidth="22400" windowHeight="13600" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
+    <workbookView xWindow="-32320" yWindow="-8380" windowWidth="22400" windowHeight="13600" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -123,11 +123,6 @@
     <t xml:space="preserve">Alors, on commence ! </t>
   </si>
   <si>
-    <t>R pour revenir au début des instructions
-Bienvenue à la course des champions 
-Merci d'avoir rejoint le jury !</t>
-  </si>
-  <si>
     <t>Voici une série de sauts réguliers.
 Tu vas entendre le bruit des sauts de Bunny. 
 C'est comme ça que tu sauras s'il a fait des sauts bien réguliers ou pas</t>
@@ -149,6 +144,11 @@
   </si>
   <si>
     <t>Diapositive13</t>
+  </si>
+  <si>
+    <t>Espace pour revenir au début des instructions
+Bienvenue à la course des champions 
+Merci d'avoir rejoint le jury !</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -742,26 +742,26 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new slides provided by Rita
</commit_message>
<xml_diff>
--- a/stories/Bunny/story.xlsx
+++ b/stories/Bunny/story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheylus/Documents/Rita/PythonMLP_2024_PAMCAP_EPCT_Rita/stories/Bunny/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAM\Documents\dycg_users\RITA\PythonMLP_2024_PAMCAP_EPCT_Rita-RabbitsVersion\stories\Bunny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F63282-B743-304B-9586-463C33DF2508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D3E05-F5F9-4909-8F1C-6A6684108ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32320" yWindow="-8380" windowWidth="22400" windowHeight="13600" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
+    <workbookView xWindow="6840" yWindow="3045" windowWidth="21600" windowHeight="11295" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Type</t>
   </si>
@@ -149,13 +139,27 @@
     <t>Espace pour revenir au début des instructions
 Bienvenue à la course des champions 
 Merci d'avoir rejoint le jury !</t>
+  </si>
+  <si>
+    <t>Diapositive6b</t>
+  </si>
+  <si>
+    <t>Diapositive6c</t>
+  </si>
+  <si>
+    <t>Dans ce qui suit tu vas bien entendre les sauts
+et essayer d'appuyer sur la bonne touche.</t>
+  </si>
+  <si>
+    <t>Si la première fois tu n'as pas bien entendu les sauts, tu peux réécouter
+en appuyant sur ESPACE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +169,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,9 +201,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -509,20 +526,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CA3E0B-1C38-6740-ADF8-D4AD5FF5992A}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -573,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -590,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -607,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -624,7 +641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -641,131 +658,166 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Full-screen slides on PAM_STIM_2024
</commit_message>
<xml_diff>
--- a/stories/Bunny/story.xlsx
+++ b/stories/Bunny/story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAM\Documents\dycg_users\RITA\PythonMLP_2024_PAMCAP_EPCT_Rita-RabbitsVersion\stories\Bunny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Ultra Touch/RITA/MLPStory4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D3E05-F5F9-4909-8F1C-6A6684108ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6505D4-B0C5-C044-B061-8263A379ADE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="3045" windowWidth="21600" windowHeight="11295" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
+    <workbookView xWindow="15300" yWindow="13040" windowWidth="31640" windowHeight="17380" xr2:uid="{8FAE3BAC-2847-E54B-870A-D43C50EBCF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Diapositive6</t>
   </si>
   <si>
-    <t>Diapositive10</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Bloc</t>
   </si>
   <si>
-    <t>Diapositive11</t>
-  </si>
-  <si>
     <t>Diapositive12</t>
   </si>
   <si>
@@ -141,18 +135,24 @@
 Merci d'avoir rejoint le jury !</t>
   </si>
   <si>
-    <t>Diapositive6b</t>
-  </si>
-  <si>
-    <t>Diapositive6c</t>
-  </si>
-  <si>
     <t>Dans ce qui suit tu vas bien entendre les sauts
 et essayer d'appuyer sur la bonne touche.</t>
   </si>
   <si>
     <t>Si la première fois tu n'as pas bien entendu les sauts, tu peux réécouter
 en appuyant sur ESPACE</t>
+  </si>
+  <si>
+    <t>Diapositive7</t>
+  </si>
+  <si>
+    <t>Diapositive8</t>
+  </si>
+  <si>
+    <t>Diapositive14</t>
+  </si>
+  <si>
+    <t>Diapositive15</t>
   </si>
 </sst>
 </file>
@@ -529,17 +529,17 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,12 +556,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -573,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -590,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -607,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -624,12 +624,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -641,7 +641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -658,12 +658,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -675,12 +675,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
@@ -692,12 +692,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -709,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -726,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -743,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -760,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -777,39 +777,39 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>

</xml_diff>